<commit_message>
Update of the code with the latests estimates
These updates work with Daria's new estimates for the UK.
</commit_message>
<xml_diff>
--- a/input/DatabaseCountryYear.xlsx
+++ b/input/DatabaseCountryYear.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="755" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1319" uniqueCount="9">
   <si>
     <t>Country</t>
   </si>
@@ -57,6 +57,9 @@
   </si>
   <si>
     <t>2019</t>
+  </si>
+  <si>
+    <t>2015</t>
   </si>
 </sst>
 </file>
@@ -428,7 +431,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>